<commit_message>
Add more historic revenue data
</commit_message>
<xml_diff>
--- a/data/reddit-monthly-revenue-report.xlsx
+++ b/data/reddit-monthly-revenue-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhuo En Tan\Desktop\ML\blue-archive-forecasting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18C4681-A654-46AB-9C5B-C028D1CD12CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FE8532-2416-4754-84AA-8373C7A97DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="16200" windowHeight="9307" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,10 @@
     <t>2023-01 to 2024-10: from u/numberlockbs</t>
   </si>
   <si>
-    <t>2022-10 to 2022-12: from u/visiroth</t>
+    <t>* using 2024-07 data from the 2024-08 post</t>
   </si>
   <si>
-    <t>* using 2024-07 data from the 2024-08 post</t>
+    <t>2022-12 and prior: from u/mee8Ti6Eit</t>
   </si>
 </sst>
 </file>
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -466,80 +466,122 @@
       <c r="A11" s="1">
         <v>44501</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>3000000</v>
+      </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>44531</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>2000000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5000000</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>44562</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="2">
+        <v>6000000</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2800000</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>44593</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2">
+        <v>4000000</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2800000</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>44621</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2">
+        <v>2000000</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2700000</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>44652</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B16" s="2">
+        <v>1900000</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>44682</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B17" s="2">
+        <v>2000000</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2900000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>44713</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B18" s="2">
+        <v>4000000</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>44743</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B19" s="2">
+        <v>10000000</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>44774</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B20" s="2">
+        <v>6989822</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1058556</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>44805</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B21" s="2">
+        <v>4000000</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>44835</v>
       </c>
@@ -549,22 +591,19 @@
       <c r="C22" s="2">
         <v>1500000</v>
       </c>
-      <c r="E22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>44866</v>
       </c>
       <c r="B23" s="2">
-        <v>4000000</v>
+        <v>5000000</v>
       </c>
       <c r="C23" s="2">
         <v>1500000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>44896</v>
       </c>
@@ -574,8 +613,11 @@
       <c r="C24" s="2">
         <v>1500000</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>44927</v>
       </c>
@@ -585,11 +627,11 @@
       <c r="C25" s="2">
         <v>2700000</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>44958</v>
       </c>
@@ -600,7 +642,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>44986</v>
       </c>
@@ -611,7 +653,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>45017</v>
       </c>
@@ -622,7 +664,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>45047</v>
       </c>
@@ -633,7 +675,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>45078</v>
       </c>
@@ -644,7 +686,7 @@
         <v>1700000</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>45108</v>
       </c>
@@ -655,7 +697,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>45139</v>
       </c>
@@ -666,7 +708,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>45170</v>
       </c>
@@ -677,7 +719,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>45200</v>
       </c>
@@ -688,7 +730,7 @@
         <v>1700000</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>45231</v>
       </c>
@@ -699,7 +741,7 @@
         <v>2900000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>45261</v>
       </c>
@@ -710,7 +752,7 @@
         <v>1600000</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>45292</v>
       </c>
@@ -721,7 +763,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>45323</v>
       </c>
@@ -732,7 +774,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>45352</v>
       </c>
@@ -743,7 +785,7 @@
         <v>1700000</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>45383</v>
       </c>
@@ -754,7 +796,7 @@
         <v>1700000</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>45413</v>
       </c>
@@ -765,7 +807,7 @@
         <v>2800000</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>45444</v>
       </c>
@@ -776,7 +818,7 @@
         <v>2700000</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>45474</v>
       </c>
@@ -786,11 +828,11 @@
       <c r="C43" s="2">
         <v>3000000</v>
       </c>
-      <c r="E43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>45505</v>
       </c>
@@ -801,7 +843,7 @@
         <v>3800000</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>45536</v>
       </c>
@@ -812,7 +854,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>45566</v>
       </c>
@@ -823,12 +865,12 @@
         <v>2700000</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>

</xml_diff>

<commit_message>
Clear excel formatting to improve loading speed
reddit-monthly-revenue-report.xlsx and revenue-ennead-cc-revenue-report.xlsx were reformatted.
</commit_message>
<xml_diff>
--- a/data/reddit-monthly-revenue-report.xlsx
+++ b/data/reddit-monthly-revenue-report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhuo En Tan\Desktop\ML\blue-archive-forecasting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FE8532-2416-4754-84AA-8373C7A97DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CF9917-52E5-4ABD-A75E-B068A36C46FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="16200" windowHeight="9307" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6645" yWindow="2393" windowWidth="16200" windowHeight="9307" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,22 +27,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>JP</t>
   </si>
   <si>
     <t>Global</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>2022-12 and prior: from u/mee8Ti6Eit</t>
   </si>
   <si>
     <t>2023-01 to 2024-10: from u/numberlockbs</t>
   </si>
   <si>
     <t>* using 2024-07 data from the 2024-08 post</t>
-  </si>
-  <si>
-    <t>2022-12 and prior: from u/mee8Ti6Eit</t>
   </si>
 </sst>
 </file>
@@ -100,18 +100,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9CC8B6D-8A8A-44D2-8A17-1D7A9C2C2A7E}" name="Table1" displayName="Table1" ref="A1:C1048576" totalsRowShown="0">
-  <autoFilter ref="A1:C1048576" xr:uid="{C9CC8B6D-8A8A-44D2-8A17-1D7A9C2C2A7E}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{289A7C12-9497-4CBF-9804-2B045D5514CF}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{77032E17-9919-486C-81DA-9E044856AE14}" name="JP"/>
-    <tableColumn id="3" xr3:uid="{B9E985D4-74BB-4A99-9724-269499B1382C}" name="Global"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,26 +365,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -614,7 +606,7 @@
         <v>1500000</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -628,7 +620,7 @@
         <v>2700000</v>
       </c>
       <c r="F25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -829,7 +821,7 @@
         <v>3000000</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
@@ -865,180 +857,7 @@
         <v>2700000</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>